<commit_message>
Doxygen has been defeated
</commit_message>
<xml_diff>
--- a/Documentation/TEAM_GRANT_BACKLOGS.xlsx
+++ b/Documentation/TEAM_GRANT_BACKLOGS.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="59">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Make our initial setup more portable (preferably a single install script)</t>
+  </si>
+  <si>
+    <t>Find a better way to do Python documentation</t>
   </si>
 </sst>
 </file>
@@ -548,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,11 +843,11 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>36</v>
+      <c r="A30" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
         <v>40</v>
@@ -855,35 +858,35 @@
         <v>36</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10" t="s">
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>24</v>
+      <c r="B34" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
@@ -891,10 +894,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
         <v>41</v>
@@ -902,55 +905,55 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="B38" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="1" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="10" t="s">
+    <row r="40" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+      <c r="B40" s="10" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>29</v>
+      <c r="B41" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C41" t="s">
         <v>41</v>
@@ -961,27 +964,27 @@
         <v>36</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="10" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+      <c r="B44" s="10" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C44" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,27 +992,27 @@
         <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="10" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="10" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,9 +1020,20 @@
         <v>36</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>